<commit_message>
dynamic member role set up
</commit_message>
<xml_diff>
--- a/public/templates/members_bulk_template.xlsx
+++ b/public/templates/members_bulk_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thetnaungsoe/Desktop/ChronoFlow-Registration/ChronoFlow-Frontend/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3333362-1124-D34B-9F00-1B67C6B8A1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FEAEBF-8BF3-C247-A5A5-D699A0B91FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{89549748-427B-B94C-86B8-0C892B28E151}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>email</t>
   </si>
   <si>
-    <t>roleIds</t>
+    <t>remark</t>
   </si>
   <si>
-    <t>remark</t>
+    <t>roleKeys</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,10 +409,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>